<commit_message>
Port as far as tileIntersectsRowProcessing
</commit_message>
<xml_diff>
--- a/Progress Reports/CDC Monthly progress reports/2016/CDC RIF plans - July to December 2016.xlsx
+++ b/Progress Reports/CDC Monthly progress reports/2016/CDC RIF plans - July to December 2016.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17426"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="6640" activeTab="1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="238">
   <si>
     <t>Details</t>
   </si>
@@ -592,9 +592,6 @@
   </si>
   <si>
     <t>Handover to new GIS person</t>
-  </si>
-  <si>
-    <t>Not allocated (for overrun)</t>
   </si>
   <si>
     <t>Data Viewer</t>
@@ -688,9 +685,6 @@
     <t>October to December</t>
   </si>
   <si>
-    <t>Not allocated (for overrun - 15 days)</t>
-  </si>
-  <si>
     <t>MD</t>
   </si>
   <si>
@@ -754,22 +748,40 @@
     <t>Documentation, manual</t>
   </si>
   <si>
-    <t>Final Integration</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Not allocated (for overrun): now 3.4 Performance scaleability (8 days) </t>
-  </si>
-  <si>
     <t>Not allocated (for overrun - 9 days): now map tile generation</t>
   </si>
   <si>
     <t>Not allocated (for overrun - 10 days): now data viewer get methods</t>
   </si>
   <si>
-    <t>Not allocated (for overrun): now data loader</t>
-  </si>
-  <si>
     <t>SQL Server study submission and data extraction</t>
+  </si>
+  <si>
+    <t>CDC Visit</t>
+  </si>
+  <si>
+    <t>Java handover, fix submission feature</t>
+  </si>
+  <si>
+    <t>Calling R; end to end; submission feature</t>
+  </si>
+  <si>
+    <t>ALPSAC</t>
+  </si>
+  <si>
+    <t>Disease Mapping</t>
+  </si>
+  <si>
+    <t>SQL Server middleware</t>
+  </si>
+  <si>
+    <t>Reamaining data display methods</t>
+  </si>
+  <si>
+    <t>Unallocated</t>
+  </si>
+  <si>
+    <t>SQL Server tile integration</t>
   </si>
 </sst>
 </file>
@@ -824,7 +836,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -834,6 +846,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -850,7 +868,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -977,26 +995,45 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1432,7 +1469,7 @@
         <v>42594</v>
       </c>
       <c r="H3" s="14" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="I3" s="8">
         <v>42552</v>
@@ -1491,7 +1528,7 @@
       </c>
       <c r="K5" s="8"/>
       <c r="L5" s="7" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="58" x14ac:dyDescent="0.35">
@@ -1582,7 +1619,7 @@
         <v>42616</v>
       </c>
       <c r="H8" s="14" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="I8" s="8">
         <v>42583</v>
@@ -1592,7 +1629,7 @@
       </c>
       <c r="K8" s="6"/>
       <c r="L8" s="33" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.35">
@@ -1663,7 +1700,7 @@
     </row>
     <row r="12" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="A12" s="6" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
@@ -1700,7 +1737,7 @@
     </row>
     <row r="13" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="A13" s="6" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -1847,7 +1884,7 @@
       <c r="J18" s="6"/>
       <c r="K18" s="6"/>
       <c r="L18" s="7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.35">
@@ -1855,7 +1892,7 @@
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E19" s="6" t="s">
         <v>51</v>
@@ -1869,7 +1906,7 @@
       <c r="J19" s="6"/>
       <c r="K19" s="6"/>
       <c r="L19" s="7" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.35">
@@ -2016,7 +2053,7 @@
     </row>
     <row r="27" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="A27" s="6" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B27" s="6"/>
       <c r="C27" s="6" t="s">
@@ -2035,7 +2072,7 @@
       <c r="J27" s="6"/>
       <c r="K27" s="12"/>
       <c r="L27" s="7" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="28" spans="1:12" ht="29" x14ac:dyDescent="0.35">
@@ -2043,7 +2080,7 @@
       <c r="B28" s="6"/>
       <c r="C28" s="6"/>
       <c r="D28" s="6" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E28" s="6"/>
       <c r="F28" s="6"/>
@@ -2536,11 +2573,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I31"/>
+  <dimension ref="A1:I38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C25" sqref="C25:G25"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C24" sqref="C24:C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2572,7 +2609,7 @@
         <v>17</v>
       </c>
       <c r="G1" s="28" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="H1" s="5" t="s">
         <v>20</v>
@@ -2589,16 +2626,16 @@
         <f>DATE(2016,1,-2)-WEEKDAY(DATE(2016,1,3))+A3*7</f>
         <v>42555</v>
       </c>
-      <c r="C3" s="41" t="s">
+      <c r="C3" s="44" t="s">
         <v>178</v>
       </c>
       <c r="D3" s="21" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E3" s="29" t="s">
-        <v>190</v>
-      </c>
-      <c r="F3" s="47" t="s">
+        <v>189</v>
+      </c>
+      <c r="F3" s="48" t="s">
         <v>182</v>
       </c>
       <c r="G3" s="32"/>
@@ -2612,11 +2649,11 @@
         <f t="shared" ref="B4:B28" si="0">DATE(2016,1,-2)-WEEKDAY(DATE(2016,1,3))+A4*7</f>
         <v>42562</v>
       </c>
-      <c r="C4" s="41"/>
+      <c r="C4" s="44"/>
       <c r="E4" s="30" t="s">
         <v>187</v>
       </c>
-      <c r="F4" s="47"/>
+      <c r="F4" s="48"/>
       <c r="G4" s="32"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
@@ -2628,17 +2665,17 @@
         <f t="shared" si="0"/>
         <v>42569</v>
       </c>
-      <c r="C5" s="41"/>
+      <c r="C5" s="44"/>
       <c r="D5" s="34" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="E5" s="30" t="s">
         <v>186</v>
       </c>
-      <c r="F5" s="48" t="s">
+      <c r="F5" s="49" t="s">
         <v>184</v>
       </c>
-      <c r="G5" s="47"/>
+      <c r="G5" s="48"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="37">
@@ -2649,15 +2686,15 @@
         <f t="shared" si="0"/>
         <v>42576</v>
       </c>
-      <c r="C6" s="41"/>
+      <c r="C6" s="44"/>
       <c r="D6" s="21" t="s">
         <v>27</v>
       </c>
       <c r="E6" s="40" t="s">
-        <v>215</v>
-      </c>
-      <c r="F6" s="48"/>
-      <c r="G6" s="47"/>
+        <v>213</v>
+      </c>
+      <c r="F6" s="49"/>
+      <c r="G6" s="48"/>
       <c r="H6" s="6" t="s">
         <v>74</v>
       </c>
@@ -2671,19 +2708,19 @@
         <f t="shared" si="0"/>
         <v>42583</v>
       </c>
-      <c r="C7" s="41" t="s">
+      <c r="C7" s="44" t="s">
         <v>179</v>
       </c>
-      <c r="D7" s="41" t="s">
+      <c r="D7" s="44" t="s">
         <v>182</v>
       </c>
       <c r="E7" s="30" t="s">
         <v>188</v>
       </c>
-      <c r="F7" s="41" t="s">
+      <c r="F7" s="44" t="s">
         <v>182</v>
       </c>
-      <c r="G7" s="47"/>
+      <c r="G7" s="48"/>
     </row>
     <row r="8" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="37">
@@ -2694,13 +2731,13 @@
         <f t="shared" si="0"/>
         <v>42590</v>
       </c>
-      <c r="C8" s="41"/>
-      <c r="D8" s="43"/>
+      <c r="C8" s="44"/>
+      <c r="D8" s="45"/>
       <c r="E8" s="40" t="s">
-        <v>212</v>
-      </c>
-      <c r="F8" s="45"/>
-      <c r="G8" s="47"/>
+        <v>210</v>
+      </c>
+      <c r="F8" s="46"/>
+      <c r="G8" s="48"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="37">
@@ -2714,16 +2751,16 @@
       <c r="C9" s="39" t="s">
         <v>184</v>
       </c>
-      <c r="D9" s="41" t="s">
-        <v>222</v>
+      <c r="D9" s="44" t="s">
+        <v>220</v>
       </c>
       <c r="E9" s="39" t="s">
         <v>184</v>
       </c>
-      <c r="F9" s="48" t="s">
+      <c r="F9" s="49" t="s">
         <v>184</v>
       </c>
-      <c r="G9" s="47"/>
+      <c r="G9" s="48"/>
     </row>
     <row r="10" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="37">
@@ -2735,14 +2772,14 @@
         <v>42604</v>
       </c>
       <c r="C10" s="27" t="s">
-        <v>209</v>
-      </c>
-      <c r="D10" s="41"/>
+        <v>207</v>
+      </c>
+      <c r="D10" s="44"/>
       <c r="E10" s="29" t="s">
-        <v>192</v>
-      </c>
-      <c r="F10" s="48"/>
-      <c r="G10" s="47"/>
+        <v>191</v>
+      </c>
+      <c r="F10" s="49"/>
+      <c r="G10" s="48"/>
     </row>
     <row r="11" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A11" s="37">
@@ -2753,21 +2790,21 @@
         <f t="shared" si="0"/>
         <v>42611</v>
       </c>
-      <c r="C11" s="41" t="s">
-        <v>202</v>
-      </c>
-      <c r="D11" s="41"/>
+      <c r="C11" s="44" t="s">
+        <v>201</v>
+      </c>
+      <c r="D11" s="44"/>
       <c r="E11" s="27" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="F11" s="29" t="s">
         <v>185</v>
       </c>
       <c r="G11" s="30" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="H11" s="6" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
@@ -2779,15 +2816,15 @@
         <f t="shared" si="0"/>
         <v>42618</v>
       </c>
-      <c r="C12" s="43"/>
-      <c r="D12" s="41" t="s">
-        <v>231</v>
+      <c r="C12" s="45"/>
+      <c r="D12" s="44" t="s">
+        <v>227</v>
       </c>
       <c r="E12" s="31" t="s">
-        <v>191</v>
-      </c>
-      <c r="F12" s="46" t="s">
-        <v>211</v>
+        <v>190</v>
+      </c>
+      <c r="F12" s="47" t="s">
+        <v>209</v>
       </c>
       <c r="G12" s="21" t="s">
         <v>183</v>
@@ -2802,16 +2839,16 @@
         <f t="shared" si="0"/>
         <v>42625</v>
       </c>
-      <c r="C13" s="41" t="s">
-        <v>201</v>
-      </c>
-      <c r="D13" s="41"/>
-      <c r="E13" s="41" t="s">
-        <v>220</v>
-      </c>
-      <c r="F13" s="43"/>
-      <c r="G13" s="41" t="s">
-        <v>226</v>
+      <c r="C13" s="44" t="s">
+        <v>200</v>
+      </c>
+      <c r="D13" s="44"/>
+      <c r="E13" s="44" t="s">
+        <v>218</v>
+      </c>
+      <c r="F13" s="45"/>
+      <c r="G13" s="44" t="s">
+        <v>224</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
@@ -2823,13 +2860,13 @@
         <f t="shared" si="0"/>
         <v>42632</v>
       </c>
-      <c r="C14" s="41"/>
-      <c r="D14" s="42" t="s">
-        <v>196</v>
-      </c>
-      <c r="E14" s="41"/>
-      <c r="F14" s="43"/>
-      <c r="G14" s="41"/>
+      <c r="C14" s="44"/>
+      <c r="D14" s="50" t="s">
+        <v>195</v>
+      </c>
+      <c r="E14" s="44"/>
+      <c r="F14" s="45"/>
+      <c r="G14" s="44"/>
       <c r="H14" s="6" t="s">
         <v>73</v>
       </c>
@@ -2843,13 +2880,13 @@
         <f t="shared" si="0"/>
         <v>42639</v>
       </c>
-      <c r="C15" s="41" t="s">
-        <v>203</v>
-      </c>
-      <c r="D15" s="41"/>
-      <c r="E15" s="41"/>
-      <c r="F15" s="43"/>
-      <c r="G15" s="41"/>
+      <c r="C15" s="44" t="s">
+        <v>202</v>
+      </c>
+      <c r="D15" s="44"/>
+      <c r="E15" s="44"/>
+      <c r="F15" s="45"/>
+      <c r="G15" s="44"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" s="37">
@@ -2860,13 +2897,15 @@
         <f t="shared" si="0"/>
         <v>42646</v>
       </c>
-      <c r="C16" s="41"/>
-      <c r="D16" s="41"/>
+      <c r="C16" s="44"/>
+      <c r="D16" s="44" t="s">
+        <v>231</v>
+      </c>
       <c r="E16" s="31" t="s">
-        <v>191</v>
-      </c>
-      <c r="F16" s="43"/>
-      <c r="G16" s="41"/>
+        <v>190</v>
+      </c>
+      <c r="F16" s="45"/>
+      <c r="G16" s="44"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" s="37">
@@ -2877,17 +2916,15 @@
         <f t="shared" si="0"/>
         <v>42653</v>
       </c>
-      <c r="C17" s="41" t="s">
-        <v>230</v>
-      </c>
-      <c r="D17" s="41" t="s">
-        <v>223</v>
-      </c>
-      <c r="E17" s="41" t="s">
-        <v>220</v>
-      </c>
-      <c r="F17" s="43"/>
-      <c r="G17" s="41"/>
+      <c r="C17" s="44" t="s">
+        <v>226</v>
+      </c>
+      <c r="D17" s="45"/>
+      <c r="E17" s="44" t="s">
+        <v>218</v>
+      </c>
+      <c r="F17" s="45"/>
+      <c r="G17" s="44"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" s="37">
@@ -2898,11 +2935,11 @@
         <f t="shared" si="0"/>
         <v>42660</v>
       </c>
-      <c r="C18" s="41"/>
-      <c r="D18" s="43"/>
-      <c r="E18" s="41"/>
-      <c r="F18" s="43"/>
-      <c r="G18" s="41"/>
+      <c r="C18" s="44"/>
+      <c r="D18" s="45"/>
+      <c r="E18" s="44"/>
+      <c r="F18" s="45"/>
+      <c r="G18" s="44"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" s="37">
@@ -2913,11 +2950,11 @@
         <f t="shared" si="0"/>
         <v>42667</v>
       </c>
-      <c r="C19" s="41"/>
-      <c r="D19" s="43"/>
-      <c r="E19" s="41"/>
-      <c r="F19" s="43"/>
-      <c r="G19" s="41"/>
+      <c r="C19" s="44"/>
+      <c r="D19" s="45"/>
+      <c r="E19" s="44"/>
+      <c r="F19" s="45"/>
+      <c r="G19" s="44"/>
     </row>
     <row r="20" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="37">
@@ -2928,17 +2965,15 @@
         <f t="shared" si="0"/>
         <v>42674</v>
       </c>
-      <c r="C20" s="41" t="s">
-        <v>233</v>
-      </c>
-      <c r="D20" s="43"/>
+      <c r="C20" s="45"/>
+      <c r="D20" s="39" t="s">
+        <v>232</v>
+      </c>
       <c r="E20" s="31" t="s">
-        <v>191</v>
-      </c>
-      <c r="F20" s="43" t="s">
-        <v>227</v>
-      </c>
-      <c r="G20" s="41"/>
+        <v>190</v>
+      </c>
+      <c r="F20" s="46"/>
+      <c r="G20" s="44"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" s="37">
@@ -2949,13 +2984,15 @@
         <f t="shared" si="0"/>
         <v>42681</v>
       </c>
-      <c r="C21" s="41"/>
-      <c r="D21" s="43"/>
-      <c r="E21" s="41" t="s">
-        <v>206</v>
-      </c>
-      <c r="F21" s="45"/>
-      <c r="G21" s="41"/>
+      <c r="C21" s="45"/>
+      <c r="D21" s="41" t="s">
+        <v>230</v>
+      </c>
+      <c r="E21" s="44" t="s">
+        <v>233</v>
+      </c>
+      <c r="F21" s="46"/>
+      <c r="G21" s="44"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" s="37">
@@ -2966,11 +3003,13 @@
         <f t="shared" si="0"/>
         <v>42688</v>
       </c>
-      <c r="C22" s="41"/>
-      <c r="D22" s="43"/>
-      <c r="E22" s="41"/>
-      <c r="F22" s="45"/>
-      <c r="G22" s="41"/>
+      <c r="C22" s="45"/>
+      <c r="D22" s="39" t="s">
+        <v>184</v>
+      </c>
+      <c r="E22" s="44"/>
+      <c r="F22" s="46"/>
+      <c r="G22" s="44"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" s="37">
@@ -2981,11 +3020,13 @@
         <f t="shared" si="0"/>
         <v>42695</v>
       </c>
-      <c r="C23" s="41"/>
-      <c r="D23" s="43"/>
-      <c r="E23" s="43"/>
-      <c r="F23" s="45"/>
-      <c r="G23" s="41"/>
+      <c r="C23" s="45"/>
+      <c r="D23" s="41" t="s">
+        <v>230</v>
+      </c>
+      <c r="E23" s="45"/>
+      <c r="F23" s="46"/>
+      <c r="G23" s="44"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" s="37">
@@ -2996,13 +3037,17 @@
         <f t="shared" si="0"/>
         <v>42702</v>
       </c>
-      <c r="C24" s="41"/>
-      <c r="D24" s="43"/>
+      <c r="C24" s="44" t="s">
+        <v>237</v>
+      </c>
+      <c r="D24" s="44" t="s">
+        <v>221</v>
+      </c>
       <c r="E24" s="31" t="s">
-        <v>191</v>
-      </c>
-      <c r="F24" s="45"/>
-      <c r="G24" s="41"/>
+        <v>190</v>
+      </c>
+      <c r="F24" s="46"/>
+      <c r="G24" s="44"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" s="37">
@@ -3013,13 +3058,15 @@
         <f t="shared" si="0"/>
         <v>42709</v>
       </c>
-      <c r="C25" s="44" t="s">
-        <v>228</v>
-      </c>
-      <c r="D25" s="44"/>
-      <c r="E25" s="44"/>
-      <c r="F25" s="44"/>
-      <c r="G25" s="44"/>
+      <c r="C25" s="44"/>
+      <c r="D25" s="45"/>
+      <c r="E25" s="48" t="s">
+        <v>235</v>
+      </c>
+      <c r="F25" s="46"/>
+      <c r="G25" s="48" t="s">
+        <v>234</v>
+      </c>
       <c r="H25" s="6" t="s">
         <v>72</v>
       </c>
@@ -3033,21 +3080,11 @@
         <f t="shared" si="0"/>
         <v>42716</v>
       </c>
-      <c r="C26" s="41" t="s">
-        <v>229</v>
-      </c>
-      <c r="D26" s="41" t="s">
-        <v>232</v>
-      </c>
-      <c r="E26" s="41" t="s">
-        <v>189</v>
-      </c>
-      <c r="F26" s="41" t="s">
-        <v>189</v>
-      </c>
-      <c r="G26" s="41" t="s">
-        <v>189</v>
-      </c>
+      <c r="C26" s="44"/>
+      <c r="D26" s="45"/>
+      <c r="E26" s="48"/>
+      <c r="F26" s="46"/>
+      <c r="G26" s="48"/>
       <c r="H26" s="6" t="s">
         <v>71</v>
       </c>
@@ -3061,11 +3098,13 @@
         <f t="shared" si="0"/>
         <v>42723</v>
       </c>
-      <c r="C27" s="41"/>
-      <c r="D27" s="41"/>
-      <c r="E27" s="41"/>
-      <c r="F27" s="41"/>
-      <c r="G27" s="41"/>
+      <c r="C27" s="39" t="s">
+        <v>184</v>
+      </c>
+      <c r="D27" s="45"/>
+      <c r="E27" s="48"/>
+      <c r="F27" s="46"/>
+      <c r="G27" s="48"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28" s="37">
@@ -3076,17 +3115,17 @@
         <f t="shared" si="0"/>
         <v>42730</v>
       </c>
-      <c r="C28" s="41" t="s">
-        <v>224</v>
-      </c>
-      <c r="D28" s="41"/>
-      <c r="E28" s="41"/>
-      <c r="F28" s="41"/>
-      <c r="G28" s="41"/>
-      <c r="H28" s="41"/>
-      <c r="I28" s="41"/>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="C28" s="53" t="s">
+        <v>222</v>
+      </c>
+      <c r="D28" s="53"/>
+      <c r="E28" s="53"/>
+      <c r="F28" s="53"/>
+      <c r="G28" s="53"/>
+      <c r="H28" s="53"/>
+      <c r="I28" s="53"/>
+    </row>
+    <row r="29" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="37">
         <v>1</v>
       </c>
@@ -3094,28 +3133,159 @@
         <f>DATE(2017,1,-2)-WEEKDAY(DATE(2017,1,3))+A29*7</f>
         <v>42737</v>
       </c>
+      <c r="C29" s="44" t="s">
+        <v>228</v>
+      </c>
+      <c r="D29" s="44" t="s">
+        <v>221</v>
+      </c>
+      <c r="E29" s="48" t="s">
+        <v>236</v>
+      </c>
+      <c r="F29" s="45" t="s">
+        <v>225</v>
+      </c>
+      <c r="G29" s="48" t="s">
+        <v>234</v>
+      </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="D30" s="27"/>
+      <c r="A30" s="37">
+        <v>2</v>
+      </c>
+      <c r="B30" s="38">
+        <f>DATE(2017,1,-2)-WEEKDAY(DATE(2017,1,3))+A30*7</f>
+        <v>42744</v>
+      </c>
+      <c r="C30" s="44"/>
+      <c r="D30" s="55"/>
+      <c r="E30" s="54"/>
+      <c r="F30" s="46"/>
+      <c r="G30" s="48"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="C31" s="21" t="s">
-        <v>204</v>
-      </c>
-      <c r="D31" s="39" t="s">
-        <v>225</v>
+      <c r="A31" s="37">
+        <v>3</v>
+      </c>
+      <c r="B31" s="38">
+        <f>DATE(2017,1,-2)-WEEKDAY(DATE(2017,1,3))+A31*7</f>
+        <v>42751</v>
+      </c>
+      <c r="C31" s="44"/>
+      <c r="D31" s="55"/>
+      <c r="E31" s="54"/>
+      <c r="F31" s="46"/>
+      <c r="G31" s="48"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A32" s="37">
+        <v>4</v>
+      </c>
+      <c r="B32" s="38">
+        <f>DATE(2017,1,-2)-WEEKDAY(DATE(2017,1,3))+A32*7</f>
+        <v>42758</v>
+      </c>
+      <c r="C32" s="44"/>
+      <c r="D32" s="55"/>
+      <c r="E32" s="54"/>
+      <c r="F32" s="46"/>
+      <c r="G32" s="54"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A33" s="37">
+        <v>5</v>
+      </c>
+      <c r="B33" s="38">
+        <f>DATE(2017,1,-2)-WEEKDAY(DATE(2017,1,3))+A33*7</f>
+        <v>42765</v>
+      </c>
+      <c r="C33" s="44"/>
+      <c r="D33" s="55"/>
+      <c r="E33" s="54"/>
+      <c r="F33" s="46"/>
+      <c r="G33" s="54"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A34" s="37">
+        <v>6</v>
+      </c>
+      <c r="B34" s="38">
+        <f>DATE(2017,1,-2)-WEEKDAY(DATE(2017,1,3))+A34*7</f>
+        <v>42772</v>
+      </c>
+      <c r="C34" s="51" t="s">
+        <v>229</v>
+      </c>
+      <c r="D34" s="52"/>
+      <c r="E34" s="52"/>
+      <c r="F34" s="52"/>
+      <c r="G34" s="52"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A35" s="37">
+        <v>7</v>
+      </c>
+      <c r="B35" s="38">
+        <f>DATE(2017,1,-2)-WEEKDAY(DATE(2017,1,3))+A35*7</f>
+        <v>42779</v>
+      </c>
+      <c r="C35" s="42"/>
+      <c r="D35" s="42"/>
+      <c r="E35" s="43"/>
+      <c r="F35" s="43"/>
+      <c r="G35" s="43"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A36" s="37">
+        <v>8</v>
+      </c>
+      <c r="B36" s="38">
+        <f>DATE(2017,1,-2)-WEEKDAY(DATE(2017,1,3))+A36*7</f>
+        <v>42786</v>
+      </c>
+      <c r="C36" s="42"/>
+      <c r="D36" s="42"/>
+      <c r="E36" s="43"/>
+      <c r="F36" s="43"/>
+      <c r="G36" s="43"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="D37" s="27"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="C38" s="21" t="s">
+        <v>203</v>
+      </c>
+      <c r="D38" s="39" t="s">
+        <v>223</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="30">
+  <mergeCells count="32">
+    <mergeCell ref="C34:G34"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="D16:D19"/>
+    <mergeCell ref="D24:D27"/>
+    <mergeCell ref="C17:C23"/>
+    <mergeCell ref="F12:F27"/>
+    <mergeCell ref="G25:G27"/>
+    <mergeCell ref="G29:G33"/>
+    <mergeCell ref="E25:E27"/>
+    <mergeCell ref="E29:E33"/>
+    <mergeCell ref="D29:D33"/>
+    <mergeCell ref="C24:C26"/>
+    <mergeCell ref="C29:C33"/>
+    <mergeCell ref="E13:E15"/>
+    <mergeCell ref="C28:I28"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="E17:E19"/>
     <mergeCell ref="D7:D8"/>
     <mergeCell ref="D9:D11"/>
-    <mergeCell ref="C25:G25"/>
     <mergeCell ref="D12:D13"/>
     <mergeCell ref="E21:E23"/>
     <mergeCell ref="C7:C8"/>
-    <mergeCell ref="F20:F24"/>
-    <mergeCell ref="F12:F19"/>
+    <mergeCell ref="F29:F33"/>
     <mergeCell ref="C13:C14"/>
     <mergeCell ref="C15:C16"/>
     <mergeCell ref="C11:C12"/>
@@ -3124,20 +3294,6 @@
     <mergeCell ref="C3:C6"/>
     <mergeCell ref="F3:F4"/>
     <mergeCell ref="F9:F10"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="F7:F8"/>
-    <mergeCell ref="D14:D16"/>
-    <mergeCell ref="D17:D24"/>
-    <mergeCell ref="E17:E19"/>
-    <mergeCell ref="C17:C19"/>
-    <mergeCell ref="C20:C24"/>
-    <mergeCell ref="E13:E15"/>
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="C28:I28"/>
-    <mergeCell ref="D26:D27"/>
-    <mergeCell ref="E26:E27"/>
-    <mergeCell ref="F26:F27"/>
-    <mergeCell ref="G26:G27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="59" fitToHeight="0" orientation="landscape" r:id="rId1"/>

</xml_diff>